<commit_message>
AFDP-893 Create a Task CMIS Folder when task is created - code review comments - do not construct a new container folder in the AcmTask constructor
</commit_message>
<xml_diff>
--- a/acm-plugins/acm-default-plugins/acm-task-plugin/src/main/resources/rules/drools-task-rules.xlsx
+++ b/acm-plugins/acm-default-plugins/acm-task-plugin/src/main/resources/rules/drools-task-rules.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="243" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="226" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>RuleSet</t>
   </si>
@@ -31,6 +31,34 @@
     <t>com.armedia.acm.plugins.task.model.AcmTask</t>
   </si>
   <si>
+    <t>org.springframework.expression.EvaluationContext</t>
+  </si>
+  <si>
+    <t>org.springframework.expression.Expression</t>
+  </si>
+  <si>
+    <t>org.springframework.expression.ExpressionParser</t>
+  </si>
+  <si>
+    <t>org.springframework.expression.spel.standard.SpelExpressionParser</t>
+  </si>
+  <si>
+    <t>org.springframework.expression.spel.support.StandardEvaluationContext</t>
+  </si>
+  <si>
+    <t>Functions</t>
+  </si>
+  <si>
+    <t>function Boolean evalSpring(String expression, Object obj)
+{
+    ExpressionParser ep = new SpelExpressionParser();
+    Expression exp = ep.parseExpression(expression);
+    EvaluationContext ec = new StandardEvaluationContext();
+    Boolean evaluated = exp.getValue(ec, obj, Boolean.class);
+    return evaluated;
+}</t>
+  </si>
+  <si>
     <t>Sequential</t>
   </si>
   <si>
@@ -49,7 +77,7 @@
     <t>$task: AcmTask</t>
   </si>
   <si>
-    <t>$param == null</t>
+    <t>eval(evalSpring("$param", $task))</t>
   </si>
   <si>
     <t>$task.$1($2);</t>
@@ -61,7 +89,12 @@
     <t>Rule Name</t>
   </si>
   <si>
-    <t>Field is null</t>
+    <t>Expression 1
+Must be a Spring expression that evaluates to true or false.  Leave blank if not needed.</t>
+  </si>
+  <si>
+    <t>Expression 2
+Must be a Spring expression that evaluates to true or false.  Leave blank if not needed.</t>
   </si>
   <si>
     <t>Set Field Value</t>
@@ -70,7 +103,7 @@
     <t>CMIS Folder Name</t>
   </si>
   <si>
-    <t>containerFolder.cmisFolderId</t>
+    <t>containerFolder?.cmisFolderId == null</t>
   </si>
   <si>
     <t>setEcmFolderPath, '/Sites/acm/documentLibrary/Tasks/' + $task.getTaskId()</t>
@@ -164,7 +197,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right/>
@@ -219,13 +252,6 @@
       <right style="medium"/>
       <top style="thin"/>
       <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom/>
       <diagonal/>
     </border>
     <border diagonalDown="false" diagonalUp="false">
@@ -300,6 +326,10 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="4" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="5" fillId="4" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -313,10 +343,6 @@
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="8" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="9" fillId="4" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -324,23 +350,23 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="10" fillId="6" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="10" fillId="7" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="10" fillId="8" fontId="0" numFmtId="164" xfId="0">
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="9" fillId="6" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="9" fillId="7" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="9" fillId="8" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="9" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="10" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="11" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -421,10 +447,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C10" activeCellId="0" pane="topLeft" sqref="C10"/>
+      <selection activeCell="C17" activeCellId="0" pane="topLeft" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -432,8 +458,8 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4183673469388"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.2908163265306"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="108.035714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="56.5714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.6785714285714"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="58.219387755102"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
@@ -458,144 +484,226 @@
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="4">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="7" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="5">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="5"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="6">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="6">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="2"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="7">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="7">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="8">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="8">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="8"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="9">
+        <v>2</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="113.4" outlineLevel="0" r="9">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="10" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="10">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="46.25" outlineLevel="0" r="10">
-      <c r="A10" s="11" t="s">
+      <c r="D10" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="12" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="11"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="12">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="D12" s="2"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="13">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D13" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="11">
-      <c r="A11" s="1"/>
-      <c r="B11" s="15" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="14">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="15">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D15" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="12">
-      <c r="A12" s="1"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="13">
-      <c r="A13" s="1"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="14">
-      <c r="A14" s="1"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="15">
-      <c r="A15" s="1"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="16">
-      <c r="A16" s="1"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="46.25" outlineLevel="0" r="16">
+      <c r="A16" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="17">
       <c r="A17" s="1"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="18">
+      <c r="B17" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="16"/>
+      <c r="E17" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="18">
       <c r="A18" s="1"/>
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="19">
+      <c r="E18" s="15"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="19">
       <c r="A19" s="1"/>
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
       <c r="D19" s="15"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="20">
+      <c r="E19" s="15"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="20">
       <c r="A20" s="1"/>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
       <c r="D20" s="15"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="21">
+      <c r="E20" s="15"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="21">
       <c r="A21" s="1"/>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="22">
+      <c r="E21" s="15"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="22">
       <c r="A22" s="1"/>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="23">
+      <c r="A23" s="1"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="24">
+      <c r="A24" s="1"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="26">
+      <c r="A26" s="1"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="27">
+      <c r="A27" s="1"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="28">
+      <c r="A28" s="1"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>